<commit_message>
ES Excel MediaInfo表 信息生成测试
</commit_message>
<xml_diff>
--- a/module/waapi/waapi_Auto_Import_ExternalSource/ExternalSourceDefaultMedia.xlsx
+++ b/module/waapi/waapi_Auto_Import_ExternalSource/ExternalSourceDefaultMedia.xlsx
@@ -1,217 +1,179 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="28800" windowHeight="12255" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>ExternalSourceCookie</t>
-  </si>
-  <si>
-    <t>ExternalSourceName</t>
-  </si>
-  <si>
-    <t>MediaInfoId</t>
-  </si>
-  <si>
-    <t>MediaName</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="20">
     <font>
-      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <b val="1"/>
+      <color theme="3"/>
       <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
       <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <b val="1"/>
       <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <b val="1"/>
       <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -511,161 +473,162 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -719,11 +682,74 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -975,78 +1001,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="5.375" customWidth="1"/>
-    <col min="2" max="2" width="22.625" customWidth="1"/>
-    <col min="3" max="3" width="20.375" customWidth="1"/>
-    <col min="4" max="4" width="12.625" customWidth="1"/>
-    <col min="5" max="5" width="10.375" customWidth="1"/>
+    <col width="5.375" customWidth="1" style="2" min="1" max="1"/>
+    <col width="22.625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="20.375" customWidth="1" style="2" min="3" max="3"/>
+    <col width="12.625" customWidth="1" style="2" min="4" max="4"/>
+    <col width="10.375" customWidth="1" style="2" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ExternalSourceCookie</t>
+        </is>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ExternalSourceName</t>
+        </is>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>MediaInfoId</t>
+        </is>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>MediaName</t>
+        </is>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>